<commit_message>
added reference price feature
</commit_message>
<xml_diff>
--- a/sales-e2e/resources/Reprice_Data/Reference_Price_Test_Data.xlsx
+++ b/sales-e2e/resources/Reprice_Data/Reference_Price_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravipandey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravipandey/Desktop/Savages Testcafe E2E Test/sales-e2e/sales-e2e/resources/Reprice_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A82D6F-D05D-4E4D-8FEF-B64CED03B3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FCA81-247E-F946-8F2E-1D0525808D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{7D8B3CEE-CBCB-4847-B6D7-D43D76C10306}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{7D8B3CEE-CBCB-4847-B6D7-D43D76C10306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F67666-74BE-D44C-9572-815CAA621971}">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,7 +1384,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>39</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -1968,11 +1968,8 @@
       <c r="M31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N31">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
@@ -2133,7 +2130,7 @@
         <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>20</v>
@@ -2158,7 +2155,7 @@
         <v>20000</v>
       </c>
       <c r="K36" s="2">
-        <v>5746</v>
+        <v>5745.26</v>
       </c>
       <c r="L36" s="2">
         <v>6203287151</v>
@@ -2191,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>1974.0664530069998</v>
+        <v>2091</v>
       </c>
       <c r="J37" s="2">
         <v>6000</v>
@@ -3109,10 +3106,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G60" xr:uid="{2AFBA3A0-0D16-F442-AD0A-55593D4B6729}">
       <formula1>INDIRECT(M2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B60" xr:uid="{F941837D-FEEF-414E-B3E0-E5690C39D502}">
-      <formula1>INDIRECT(A2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B60 A36" xr:uid="{F941837D-FEEF-414E-B3E0-E5690C39D502}">
+      <formula1>INDIRECT(XFD2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A60" xr:uid="{A7CFD096-E964-3D47-915F-AA59B979C89A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A35 A37:A60" xr:uid="{A7CFD096-E964-3D47-915F-AA59B979C89A}">
       <formula1>"AC,AG,CE,CI,EA,EX,IE,PO,SA,TR,UN"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F60" xr:uid="{41B37BBA-310E-C940-8E5B-6ED91AD2487B}">

</xml_diff>